<commit_message>
Cleaned example + php8.3 Docker config.
</commit_message>
<xml_diff>
--- a/tests/Unit/Roster/data/cleaned_schedule.xlsx
+++ b/tests/Unit/Roster/data/cleaned_schedule.xlsx
@@ -159,19 +159,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="hh\:mm"/>
     <numFmt numFmtId="167" formatCode="h:mm"/>
     <numFmt numFmtId="168" formatCode="General"/>
     <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -653,7 +655,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1051,6 +1053,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1261,11 +1267,11 @@
   </sheetPr>
   <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z8" activeCellId="0" sqref="Z8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.79"/>
   </cols>
@@ -2462,7 +2468,7 @@
       <c r="V21" s="30"/>
       <c r="W21" s="30"/>
       <c r="X21" s="99"/>
-      <c r="Y21" s="99"/>
+      <c r="Y21" s="100"/>
       <c r="Z21" s="80" t="n">
         <v>0</v>
       </c>
@@ -2503,7 +2509,7 @@
       <c r="F22" s="77"/>
       <c r="G22" s="83"/>
       <c r="H22" s="30"/>
-      <c r="I22" s="100"/>
+      <c r="I22" s="101"/>
       <c r="J22" s="83" t="n">
         <v>0</v>
       </c>
@@ -2515,8 +2521,8 @@
         <v>0.33333333333333</v>
       </c>
       <c r="N22" s="83"/>
-      <c r="O22" s="100"/>
-      <c r="P22" s="100"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="101"/>
       <c r="Q22" s="29" t="n">
         <v>0</v>
       </c>
@@ -2529,11 +2535,11 @@
       <c r="T22" s="29" t="n">
         <v>0.33333333333333</v>
       </c>
-      <c r="U22" s="100"/>
+      <c r="U22" s="101"/>
       <c r="V22" s="49"/>
       <c r="W22" s="49"/>
       <c r="X22" s="99"/>
-      <c r="Y22" s="99"/>
+      <c r="Y22" s="100"/>
       <c r="Z22" s="83" t="n">
         <v>0.33333333333333</v>
       </c>
@@ -2555,7 +2561,7 @@
       <c r="AN22" s="76"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="101" t="n">
+      <c r="A23" s="102" t="n">
         <v>10</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -2575,7 +2581,7 @@
       </c>
       <c r="G23" s="93"/>
       <c r="H23" s="60"/>
-      <c r="I23" s="102"/>
+      <c r="I23" s="103"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="28"/>
@@ -2585,14 +2591,14 @@
       </c>
       <c r="O23" s="30"/>
       <c r="P23" s="30"/>
-      <c r="Q23" s="103"/>
+      <c r="Q23" s="104"/>
       <c r="R23" s="28"/>
       <c r="S23" s="28"/>
       <c r="T23" s="28"/>
       <c r="U23" s="30" t="n">
         <v>0.33333333333333</v>
       </c>
-      <c r="V23" s="102"/>
+      <c r="V23" s="103"/>
       <c r="W23" s="30"/>
       <c r="X23" s="29"/>
       <c r="Y23" s="29"/>
@@ -2644,7 +2650,7 @@
       </c>
       <c r="G24" s="96"/>
       <c r="H24" s="49"/>
-      <c r="I24" s="104"/>
+      <c r="I24" s="105"/>
       <c r="J24" s="57"/>
       <c r="K24" s="57"/>
       <c r="L24" s="54"/>
@@ -2661,7 +2667,7 @@
       <c r="U24" s="49" t="n">
         <v>0.83333333333333</v>
       </c>
-      <c r="V24" s="104"/>
+      <c r="V24" s="105"/>
       <c r="W24" s="49"/>
       <c r="X24" s="57"/>
       <c r="Y24" s="57"/>
@@ -2692,10 +2698,10 @@
       <c r="AN24" s="76"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="105" t="n">
+      <c r="A25" s="106" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B25" s="107" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -2745,7 +2751,7 @@
       </c>
       <c r="AD25" s="30"/>
       <c r="AE25" s="29"/>
-      <c r="AF25" s="103"/>
+      <c r="AF25" s="104"/>
       <c r="AG25" s="29"/>
       <c r="AH25" s="28"/>
       <c r="AI25" s="31"/>
@@ -2767,8 +2773,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="105"/>
-      <c r="B26" s="106"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="43"/>
       <c r="D26" s="79"/>
       <c r="E26" s="26"/>
@@ -2824,7 +2830,7 @@
       <c r="A27" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="107" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -2837,7 +2843,7 @@
         <v>0.0381944444444444</v>
       </c>
       <c r="F27" s="46"/>
-      <c r="G27" s="107"/>
+      <c r="G27" s="108"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
@@ -2883,7 +2889,7 @@
         <v>0.33333333333333</v>
       </c>
       <c r="AH27" s="29"/>
-      <c r="AI27" s="108"/>
+      <c r="AI27" s="109"/>
       <c r="AJ27" s="51"/>
       <c r="AK27" s="33" t="n">
         <f aca="false">COUNTIF(F117:AJ118, "&gt;1")</f>
@@ -2903,12 +2909,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22"/>
-      <c r="B28" s="106"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="43"/>
       <c r="D28" s="79"/>
       <c r="E28" s="26"/>
       <c r="F28" s="46"/>
-      <c r="G28" s="109"/>
+      <c r="G28" s="110"/>
       <c r="H28" s="54"/>
       <c r="I28" s="54"/>
       <c r="J28" s="54"/>
@@ -2918,7 +2924,7 @@
       <c r="N28" s="54"/>
       <c r="O28" s="54"/>
       <c r="P28" s="54"/>
-      <c r="Q28" s="103" t="n">
+      <c r="Q28" s="104" t="n">
         <v>0.83333333333333</v>
       </c>
       <c r="R28" s="96"/>
@@ -2965,13 +2971,13 @@
       <c r="A29" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="107" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="110" t="n">
+      <c r="D29" s="111" t="n">
         <v>0.5</v>
       </c>
       <c r="E29" s="26" t="n">
@@ -3018,7 +3024,7 @@
       <c r="AF29" s="68"/>
       <c r="AG29" s="68"/>
       <c r="AH29" s="29"/>
-      <c r="AI29" s="108"/>
+      <c r="AI29" s="109"/>
       <c r="AJ29" s="51"/>
       <c r="AK29" s="33" t="n">
         <f aca="false">COUNTIF(F119:AJ120, "&gt;1")</f>
@@ -3028,7 +3034,7 @@
         <f aca="false">SUM(F119:AJ120)</f>
         <v>0</v>
       </c>
-      <c r="AM29" s="111" t="n">
+      <c r="AM29" s="112" t="n">
         <f aca="false">AN29*1.85</f>
         <v>37</v>
       </c>
@@ -3038,9 +3044,9 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22"/>
-      <c r="B30" s="106"/>
+      <c r="B30" s="107"/>
       <c r="C30" s="43"/>
-      <c r="D30" s="110"/>
+      <c r="D30" s="111"/>
       <c r="E30" s="26"/>
       <c r="F30" s="77"/>
       <c r="G30" s="96"/>
@@ -3057,7 +3063,7 @@
       </c>
       <c r="O30" s="49"/>
       <c r="P30" s="49"/>
-      <c r="Q30" s="103"/>
+      <c r="Q30" s="104"/>
       <c r="R30" s="96"/>
       <c r="S30" s="57"/>
       <c r="T30" s="57" t="n">
@@ -3087,7 +3093,7 @@
       <c r="AJ30" s="63"/>
       <c r="AK30" s="33"/>
       <c r="AL30" s="34"/>
-      <c r="AM30" s="111"/>
+      <c r="AM30" s="112"/>
       <c r="AN30" s="33"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,7 +3106,7 @@
       <c r="C31" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="110" t="n">
+      <c r="D31" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E31" s="26" t="n">
@@ -3163,7 +3169,7 @@
       <c r="A32" s="22"/>
       <c r="B32" s="97"/>
       <c r="C32" s="43"/>
-      <c r="D32" s="110"/>
+      <c r="D32" s="111"/>
       <c r="E32" s="26"/>
       <c r="F32" s="77" t="n">
         <v>0.33333333333333</v>
@@ -3211,13 +3217,13 @@
       <c r="A33" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="107" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="110" t="n">
+      <c r="D33" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E33" s="26" t="n">
@@ -3276,9 +3282,9 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22"/>
-      <c r="B34" s="106"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="43"/>
-      <c r="D34" s="110"/>
+      <c r="D34" s="111"/>
       <c r="E34" s="26"/>
       <c r="F34" s="77"/>
       <c r="G34" s="57"/>
@@ -3324,13 +3330,13 @@
       <c r="A35" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="B35" s="106" t="s">
+      <c r="B35" s="107" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="110" t="n">
+      <c r="D35" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E35" s="26" t="n">
@@ -3393,9 +3399,9 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22"/>
-      <c r="B36" s="106"/>
+      <c r="B36" s="107"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="110"/>
+      <c r="D36" s="111"/>
       <c r="E36" s="26"/>
       <c r="F36" s="77" t="n">
         <v>0</v>
@@ -3445,13 +3451,13 @@
       <c r="A37" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="B37" s="106" t="s">
+      <c r="B37" s="107" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="110" t="n">
+      <c r="D37" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E37" s="26" t="n">
@@ -3512,9 +3518,9 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22"/>
-      <c r="B38" s="106"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="43"/>
-      <c r="D38" s="110"/>
+      <c r="D38" s="111"/>
       <c r="E38" s="26"/>
       <c r="F38" s="90"/>
       <c r="G38" s="54"/>
@@ -3562,13 +3568,13 @@
       <c r="A39" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="107" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="110" t="n">
+      <c r="D39" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E39" s="26" t="n">
@@ -3631,9 +3637,9 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22"/>
-      <c r="B40" s="106"/>
+      <c r="B40" s="107"/>
       <c r="C40" s="43"/>
-      <c r="D40" s="110"/>
+      <c r="D40" s="111"/>
       <c r="E40" s="26"/>
       <c r="F40" s="77"/>
       <c r="G40" s="54"/>
@@ -3683,13 +3689,13 @@
       <c r="A41" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="106" t="s">
+      <c r="B41" s="107" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="110" t="n">
+      <c r="D41" s="111" t="n">
         <v>0.25</v>
       </c>
       <c r="E41" s="26" t="n">
@@ -3744,9 +3750,9 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22"/>
-      <c r="B42" s="106"/>
+      <c r="B42" s="107"/>
       <c r="C42" s="43"/>
-      <c r="D42" s="110"/>
+      <c r="D42" s="111"/>
       <c r="E42" s="26"/>
       <c r="F42" s="77"/>
       <c r="G42" s="57"/>
@@ -3788,7 +3794,7 @@
       <c r="A43" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="106" t="s">
+      <c r="B43" s="107" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="43" t="s">
@@ -3857,12 +3863,12 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22"/>
-      <c r="B44" s="106"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="43"/>
       <c r="D44" s="25"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="113"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="114"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
       <c r="J44" s="57"/>
@@ -3909,7 +3915,7 @@
       <c r="A45" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="106" t="s">
+      <c r="B45" s="107" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="43" t="s">
@@ -3972,12 +3978,12 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22"/>
-      <c r="B46" s="106"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="43"/>
       <c r="D46" s="25"/>
       <c r="E46" s="26"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="113"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="114"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
       <c r="J46" s="57"/>
@@ -3991,8 +3997,8 @@
       <c r="P46" s="54"/>
       <c r="Q46" s="54"/>
       <c r="R46" s="54"/>
-      <c r="S46" s="114"/>
-      <c r="T46" s="115"/>
+      <c r="S46" s="115"/>
+      <c r="T46" s="116"/>
       <c r="U46" s="54"/>
       <c r="V46" s="54"/>
       <c r="W46" s="54"/>
@@ -4015,11 +4021,11 @@
       <c r="AN46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="116"/>
-      <c r="B47" s="117"/>
-      <c r="C47" s="118"/>
-      <c r="D47" s="119"/>
-      <c r="E47" s="120"/>
+      <c r="A47" s="117"/>
+      <c r="B47" s="118"/>
+      <c r="C47" s="119"/>
+      <c r="D47" s="120"/>
+      <c r="E47" s="121"/>
       <c r="F47" s="46"/>
       <c r="G47" s="29"/>
       <c r="H47" s="30"/>
@@ -4051,17 +4057,17 @@
       <c r="AH47" s="29"/>
       <c r="AI47" s="31"/>
       <c r="AJ47" s="51"/>
-      <c r="AK47" s="121"/>
-      <c r="AL47" s="122"/>
-      <c r="AM47" s="116"/>
-      <c r="AN47" s="116"/>
+      <c r="AK47" s="122"/>
+      <c r="AL47" s="123"/>
+      <c r="AM47" s="117"/>
+      <c r="AN47" s="117"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="116"/>
-      <c r="B48" s="117"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="119"/>
-      <c r="E48" s="120"/>
+      <c r="A48" s="117"/>
+      <c r="B48" s="118"/>
+      <c r="C48" s="119"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="121"/>
       <c r="F48" s="77"/>
       <c r="G48" s="57"/>
       <c r="H48" s="49"/>
@@ -4093,54 +4099,54 @@
       <c r="AH48" s="57"/>
       <c r="AI48" s="62"/>
       <c r="AJ48" s="63"/>
-      <c r="AK48" s="121"/>
-      <c r="AL48" s="122"/>
-      <c r="AM48" s="116"/>
-      <c r="AN48" s="116"/>
+      <c r="AK48" s="122"/>
+      <c r="AL48" s="123"/>
+      <c r="AM48" s="117"/>
+      <c r="AN48" s="117"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="123"/>
-      <c r="B49" s="124"/>
-      <c r="C49" s="125"/>
-      <c r="D49" s="126"/>
-      <c r="E49" s="127" t="s">
+      <c r="A49" s="124"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="126"/>
+      <c r="D49" s="127"/>
+      <c r="E49" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="128"/>
-      <c r="G49" s="128"/>
-      <c r="H49" s="129"/>
-      <c r="I49" s="129"/>
-      <c r="J49" s="128"/>
-      <c r="K49" s="128"/>
-      <c r="L49" s="128"/>
-      <c r="M49" s="128"/>
-      <c r="N49" s="128"/>
-      <c r="O49" s="129"/>
-      <c r="P49" s="129"/>
-      <c r="Q49" s="128"/>
-      <c r="R49" s="128"/>
-      <c r="S49" s="128"/>
-      <c r="T49" s="128"/>
-      <c r="U49" s="129"/>
-      <c r="V49" s="129"/>
-      <c r="W49" s="129"/>
-      <c r="X49" s="128"/>
-      <c r="Y49" s="128"/>
-      <c r="Z49" s="128"/>
-      <c r="AA49" s="128"/>
-      <c r="AB49" s="128"/>
-      <c r="AC49" s="129"/>
-      <c r="AD49" s="129"/>
-      <c r="AE49" s="128"/>
-      <c r="AF49" s="128"/>
-      <c r="AG49" s="128"/>
-      <c r="AH49" s="128"/>
-      <c r="AI49" s="130"/>
-      <c r="AJ49" s="128"/>
-      <c r="AK49" s="123"/>
-      <c r="AL49" s="123"/>
-      <c r="AM49" s="131"/>
-      <c r="AN49" s="131"/>
+      <c r="F49" s="129"/>
+      <c r="G49" s="129"/>
+      <c r="H49" s="130"/>
+      <c r="I49" s="130"/>
+      <c r="J49" s="129"/>
+      <c r="K49" s="129"/>
+      <c r="L49" s="129"/>
+      <c r="M49" s="129"/>
+      <c r="N49" s="129"/>
+      <c r="O49" s="130"/>
+      <c r="P49" s="130"/>
+      <c r="Q49" s="129"/>
+      <c r="R49" s="129"/>
+      <c r="S49" s="129"/>
+      <c r="T49" s="129"/>
+      <c r="U49" s="130"/>
+      <c r="V49" s="130"/>
+      <c r="W49" s="130"/>
+      <c r="X49" s="129"/>
+      <c r="Y49" s="129"/>
+      <c r="Z49" s="129"/>
+      <c r="AA49" s="129"/>
+      <c r="AB49" s="129"/>
+      <c r="AC49" s="130"/>
+      <c r="AD49" s="130"/>
+      <c r="AE49" s="129"/>
+      <c r="AF49" s="129"/>
+      <c r="AG49" s="129"/>
+      <c r="AH49" s="129"/>
+      <c r="AI49" s="131"/>
+      <c r="AJ49" s="129"/>
+      <c r="AK49" s="124"/>
+      <c r="AL49" s="124"/>
+      <c r="AM49" s="132"/>
+      <c r="AN49" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="204">

</xml_diff>

<commit_message>
Summaries writting to excel.
</commit_message>
<xml_diff>
--- a/tests/Unit/Roster/data/cleaned_schedule.xlsx
+++ b/tests/Unit/Roster/data/cleaned_schedule.xlsx
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Darbo dienų</t>
   </si>
   <si>
-    <t xml:space="preserve">Darbo valan-dų</t>
+    <t xml:space="preserve">Darbo valandų priskirta</t>
   </si>
   <si>
     <t xml:space="preserve">Darbo valandų per mėnesį</t>
@@ -1267,11 +1267,11 @@
   </sheetPr>
   <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK7" activeCellId="0" sqref="AK7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.79"/>
   </cols>

</xml_diff>